<commit_message>
Defining schema for Gen1 implicits
</commit_message>
<xml_diff>
--- a/VariableStaging/Gen1Explicit.xlsx
+++ b/VariableStaging/Gen1Explicit.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gen1LivedWIthFatherAtAgeX  " sheetId="1" r:id="rId1"/>
     <sheet name="Explicit" sheetId="10" r:id="rId2"/>
+    <sheet name="ParentHealth" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="143">
   <si>
     <t>VariableCode</t>
   </si>
@@ -177,6 +178,273 @@
   </si>
   <si>
     <t>T2263800</t>
+  </si>
+  <si>
+    <t>R2837300</t>
+  </si>
+  <si>
+    <t>R2837400</t>
+  </si>
+  <si>
+    <t>R2837500</t>
+  </si>
+  <si>
+    <t>R2837600</t>
+  </si>
+  <si>
+    <t>R2837700</t>
+  </si>
+  <si>
+    <t>R2837800</t>
+  </si>
+  <si>
+    <t>R2837900</t>
+  </si>
+  <si>
+    <t>R2838000</t>
+  </si>
+  <si>
+    <t>R2838100</t>
+  </si>
+  <si>
+    <t>R2838200</t>
+  </si>
+  <si>
+    <t>R2838300</t>
+  </si>
+  <si>
+    <t>R2838400</t>
+  </si>
+  <si>
+    <t>R2838500</t>
+  </si>
+  <si>
+    <t>R2838600</t>
+  </si>
+  <si>
+    <t>R2838700</t>
+  </si>
+  <si>
+    <t>R2838800</t>
+  </si>
+  <si>
+    <t>R2838900</t>
+  </si>
+  <si>
+    <t>R2839000</t>
+  </si>
+  <si>
+    <t>R2839100</t>
+  </si>
+  <si>
+    <t>H0001600</t>
+  </si>
+  <si>
+    <t>H0013600</t>
+  </si>
+  <si>
+    <t>H0001700</t>
+  </si>
+  <si>
+    <t>H0013700</t>
+  </si>
+  <si>
+    <t>H0001800</t>
+  </si>
+  <si>
+    <t>H0001900</t>
+  </si>
+  <si>
+    <t>H0002000</t>
+  </si>
+  <si>
+    <t>H0002100</t>
+  </si>
+  <si>
+    <t>H0002200</t>
+  </si>
+  <si>
+    <t>H0002300</t>
+  </si>
+  <si>
+    <t>R0007300</t>
+  </si>
+  <si>
+    <t>H0002400</t>
+  </si>
+  <si>
+    <t>H0014700</t>
+  </si>
+  <si>
+    <t>alive 40 health</t>
+  </si>
+  <si>
+    <t>alive 50 health</t>
+  </si>
+  <si>
+    <t>deathcause 40 health</t>
+  </si>
+  <si>
+    <t>deathcause 50 health</t>
+  </si>
+  <si>
+    <t>deathage 40</t>
+  </si>
+  <si>
+    <t>deathage 50</t>
+  </si>
+  <si>
+    <t>H0013800</t>
+  </si>
+  <si>
+    <t>H0002500</t>
+  </si>
+  <si>
+    <t>H0014800</t>
+  </si>
+  <si>
+    <t>H0002600</t>
+  </si>
+  <si>
+    <t>H0014900</t>
+  </si>
+  <si>
+    <t>has probs 40</t>
+  </si>
+  <si>
+    <t>has probs 50</t>
+  </si>
+  <si>
+    <t>H0013900</t>
+  </si>
+  <si>
+    <t>H0002700</t>
+  </si>
+  <si>
+    <t>H0015000</t>
+  </si>
+  <si>
+    <t>prob1 40</t>
+  </si>
+  <si>
+    <t>prob2 40</t>
+  </si>
+  <si>
+    <t>prob3 40</t>
+  </si>
+  <si>
+    <t>prob4 40</t>
+  </si>
+  <si>
+    <t>prob1 50</t>
+  </si>
+  <si>
+    <t>prob2 50</t>
+  </si>
+  <si>
+    <t>prob3 50</t>
+  </si>
+  <si>
+    <t>prob4 50</t>
+  </si>
+  <si>
+    <t>H0014000</t>
+  </si>
+  <si>
+    <t>H0014100</t>
+  </si>
+  <si>
+    <t>H0014200</t>
+  </si>
+  <si>
+    <t>H0014300</t>
+  </si>
+  <si>
+    <t>H0014400</t>
+  </si>
+  <si>
+    <t>H0014500</t>
+  </si>
+  <si>
+    <t>prob5 50</t>
+  </si>
+  <si>
+    <t>prob6 50</t>
+  </si>
+  <si>
+    <t>prob7 50</t>
+  </si>
+  <si>
+    <t>prob8 50</t>
+  </si>
+  <si>
+    <t>prob9 50</t>
+  </si>
+  <si>
+    <t>prob10 50</t>
+  </si>
+  <si>
+    <t>H0015100</t>
+  </si>
+  <si>
+    <t>H0015200</t>
+  </si>
+  <si>
+    <t>H0015300</t>
+  </si>
+  <si>
+    <t>H0015400</t>
+  </si>
+  <si>
+    <t>H0015500</t>
+  </si>
+  <si>
+    <t>H0015600</t>
+  </si>
+  <si>
+    <t>H0015700</t>
+  </si>
+  <si>
+    <t>H0015800</t>
+  </si>
+  <si>
+    <t>H0015900</t>
+  </si>
+  <si>
+    <t>H0016000</t>
+  </si>
+  <si>
+    <t>H0002800</t>
+  </si>
+  <si>
+    <t>H0002900</t>
+  </si>
+  <si>
+    <t>H0003000</t>
+  </si>
+  <si>
+    <t>H0003100</t>
+  </si>
+  <si>
+    <t>birth country</t>
+  </si>
+  <si>
+    <t>R0006100</t>
+  </si>
+  <si>
+    <t>highest grade</t>
+  </si>
+  <si>
+    <t>R0007900</t>
+  </si>
+  <si>
+    <t>R0006500</t>
+  </si>
+  <si>
+    <t>R0007700</t>
+  </si>
+  <si>
+    <t>birth country grandfather</t>
   </si>
 </sst>
 </file>
@@ -518,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J1"/>
+      <selection activeCell="I41" sqref="A23:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,82 +1349,524 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1">
+        <v>326</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H22" s="1">
+        <v>255</v>
+      </c>
+      <c r="I22" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1">
+        <v>326</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="1">
+        <v>326</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="1">
+        <v>326</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>11</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="1">
+        <v>326</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="1">
+        <v>326</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4</v>
+      </c>
+      <c r="I27" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="1">
+        <v>326</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="1">
+        <v>326</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H29" s="1">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="1">
+        <v>326</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>11</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="I30" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="1">
+        <v>326</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H31" s="1">
+        <v>8</v>
+      </c>
+      <c r="I31" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="1">
+        <v>326</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H32">
+        <v>9</v>
+      </c>
+      <c r="I32" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="1">
+        <v>326</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H33" s="1">
+        <v>10</v>
+      </c>
+      <c r="I33" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="1">
+        <v>326</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H34">
+        <v>11</v>
+      </c>
+      <c r="I34" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="1">
+        <v>326</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H35" s="1">
+        <v>12</v>
+      </c>
+      <c r="I35" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="1">
+        <v>326</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H36">
+        <v>13</v>
+      </c>
+      <c r="I36" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="1">
+        <v>326</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H37" s="1">
+        <v>14</v>
+      </c>
+      <c r="I37" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="1">
+        <v>326</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="I38" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="1">
+        <v>326</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>11</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H39" s="1">
+        <v>16</v>
+      </c>
+      <c r="I39" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="1">
+        <v>326</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>11</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H40">
+        <v>17</v>
+      </c>
+      <c r="I40" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1">
+        <v>326</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>11</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1988</v>
+      </c>
+      <c r="H41" s="1">
+        <v>18</v>
+      </c>
+      <c r="I41" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1167,7 +1877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -1838,4 +2548,1350 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:U26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2">
+        <v>320</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>11</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3">
+        <v>320</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>11</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>301</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N4">
+        <v>321</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>11</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>301</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" t="s">
+        <v>94</v>
+      </c>
+      <c r="N5">
+        <v>321</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>302</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N6">
+        <v>322</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>302</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" t="s">
+        <v>96</v>
+      </c>
+      <c r="N7">
+        <v>322</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>11</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8">
+        <v>303</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="M8" t="s">
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <v>323</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>11</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9">
+        <v>303</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" t="s">
+        <v>101</v>
+      </c>
+      <c r="N9">
+        <v>323</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>11</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10">
+        <v>304</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10">
+        <v>324</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>11</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>304</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>103</v>
+      </c>
+      <c r="M11" t="s">
+        <v>133</v>
+      </c>
+      <c r="N11">
+        <v>324</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>11</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12">
+        <v>304</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="M12" t="s">
+        <v>134</v>
+      </c>
+      <c r="N12">
+        <v>324</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>11</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13">
+        <v>304</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13" t="s">
+        <v>135</v>
+      </c>
+      <c r="N13">
+        <v>324</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>11</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14">
+        <v>304</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" t="s">
+        <v>122</v>
+      </c>
+      <c r="N14">
+        <v>324</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15">
+        <v>304</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>107</v>
+      </c>
+      <c r="M15" t="s">
+        <v>123</v>
+      </c>
+      <c r="N15">
+        <v>324</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>11</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>6</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16">
+        <v>304</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>108</v>
+      </c>
+      <c r="M16" t="s">
+        <v>124</v>
+      </c>
+      <c r="N16">
+        <v>324</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>11</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>7</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17">
+        <v>304</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>109</v>
+      </c>
+      <c r="M17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N17">
+        <v>324</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>11</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>8</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18">
+        <v>304</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>108</v>
+      </c>
+      <c r="M18" t="s">
+        <v>126</v>
+      </c>
+      <c r="N18">
+        <v>324</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>11</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>9</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19">
+        <v>304</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>109</v>
+      </c>
+      <c r="M19" t="s">
+        <v>127</v>
+      </c>
+      <c r="N19">
+        <v>324</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>11</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>10</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>128</v>
+      </c>
+      <c r="N20">
+        <v>324</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>11</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>11</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>129</v>
+      </c>
+      <c r="N21">
+        <v>324</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>11</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>12</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>130</v>
+      </c>
+      <c r="N22">
+        <v>324</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>11</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>13</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>131</v>
+      </c>
+      <c r="N23">
+        <v>324</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>11</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>14</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24">
+        <v>305</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>11</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1979</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>136</v>
+      </c>
+      <c r="M24" t="s">
+        <v>137</v>
+      </c>
+      <c r="N24">
+        <v>325</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>11</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>1979</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25">
+        <v>307</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1979</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>138</v>
+      </c>
+      <c r="M25" t="s">
+        <v>140</v>
+      </c>
+      <c r="N25">
+        <v>327</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>11</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1979</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26">
+        <v>308</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1979</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Parents of Gen1 Retro writes to DB
</commit_message>
<xml_diff>
--- a/VariableStaging/Gen1Explicit.xlsx
+++ b/VariableStaging/Gen1Explicit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Gen1LivedWIthFatherAtAgeX  " sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="144">
   <si>
     <t>VariableCode</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>birth country grandfather</t>
+  </si>
+  <si>
+    <t>R2837200</t>
   </si>
 </sst>
 </file>
@@ -788,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I41" sqref="A23:I41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +800,7 @@
     <col min="2" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -826,13 +829,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -852,14 +854,13 @@
       <c r="I2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>11</v>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C3" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -880,12 +881,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -906,12 +907,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>13</v>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -932,12 +933,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -958,12 +959,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>15</v>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C7" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -984,12 +985,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1010,12 +1011,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>17</v>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C9" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1036,12 +1037,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1062,12 +1063,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>19</v>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1088,12 +1089,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1114,12 +1115,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>21</v>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C13" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1140,12 +1141,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1166,12 +1167,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>23</v>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C15" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1192,12 +1193,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1218,12 +1219,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>25</v>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="C17" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1244,12 +1245,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -1270,12 +1271,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>27</v>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C19" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -1296,12 +1297,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1322,12 +1323,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1348,12 +1349,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1373,13 +1375,14 @@
       <c r="I22" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -1400,12 +1403,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -1426,12 +1429,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1452,12 +1455,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1478,12 +1481,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -1504,12 +1507,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1530,12 +1533,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1556,12 +1559,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -1582,12 +1585,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1608,12 +1611,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -1636,10 +1639,10 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -1662,10 +1665,10 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -1688,10 +1691,10 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="C35" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -1714,10 +1717,10 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="C36" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -1740,10 +1743,10 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="C37" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
@@ -1766,10 +1769,10 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C38" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -1792,10 +1795,10 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
@@ -1818,10 +1821,10 @@
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="C40" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -1843,11 +1846,11 @@
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>10</v>
+      <c r="B41" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C41" s="1">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -2554,7 +2557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>

</xml_diff>